<commit_message>
Managed to get it working on a phone python compiler
</commit_message>
<xml_diff>
--- a/hello_world.xlsx
+++ b/hello_world.xlsx
@@ -443,82 +443,82 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>Weijie</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Rayshawn</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Jack</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Denver</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Ivan</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Praveen</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Junyang</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Bala</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Jinming</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Yicong</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Eugene</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Jonathan</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Alvin</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
           <t>Jowell</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Aaron</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Jonathan</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Jack</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Denver</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Max</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Ivan</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Bala</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Nigel</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Jinming</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Eugene</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>Jian Yong</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Yicong</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>Rayshawn</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>Praveen</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Junyang</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
@@ -538,37 +538,37 @@
           <t>1100-1300</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>XCBT</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t>XSVC</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -583,37 +583,37 @@
           <t>1300-1500</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>XCBT</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>XSVC</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>18</t>
         </is>
@@ -628,39 +628,39 @@
           <t>1500-1700</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
         <is>
           <t>XCBT</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>XSVC</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>CCTV</t>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
         </is>
       </c>
       <c r="S4" t="n">
@@ -673,39 +673,39 @@
           <t>1700-1900</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>XCBT</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>XSVC</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>CCTV</t>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
@@ -724,41 +724,41 @@
         </is>
       </c>
       <c r="B6" s="1" t="n"/>
-      <c r="C6" s="1" t="n"/>
-      <c r="D6" s="1" t="n"/>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
       <c r="E6" s="1" t="n"/>
-      <c r="F6" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="G6" s="1" t="n"/>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="H6" s="1" t="n"/>
-      <c r="I6" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="I6" s="1" t="n"/>
       <c r="J6" s="1" t="n"/>
       <c r="K6" s="1" t="n"/>
       <c r="L6" s="1" t="n"/>
-      <c r="M6" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="N6" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="O6" s="1" t="n"/>
-      <c r="P6" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="Q6" s="1" t="n"/>
+      <c r="M6" s="1" t="n"/>
+      <c r="N6" s="1" t="n"/>
+      <c r="O6" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="P6" s="1" t="n"/>
+      <c r="Q6" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="R6" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -775,41 +775,41 @@
         </is>
       </c>
       <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" s="1" t="n"/>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
       <c r="E7" s="1" t="n"/>
-      <c r="F7" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="G7" s="1" t="n"/>
+      <c r="F7" s="1" t="n"/>
+      <c r="G7" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="H7" s="1" t="n"/>
-      <c r="I7" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="I7" s="1" t="n"/>
       <c r="J7" s="1" t="n"/>
       <c r="K7" s="1" t="n"/>
       <c r="L7" s="1" t="n"/>
-      <c r="M7" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="N7" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="O7" s="1" t="n"/>
-      <c r="P7" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="Q7" s="1" t="n"/>
+      <c r="M7" s="1" t="n"/>
+      <c r="N7" s="1" t="n"/>
+      <c r="O7" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="P7" s="1" t="n"/>
+      <c r="Q7" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="R7" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -827,37 +827,37 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C8" s="1" t="n"/>
-      <c r="D8" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="E8" s="1" t="n"/>
-      <c r="F8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="G8" s="1" t="n"/>
       <c r="H8" s="1" t="n"/>
-      <c r="I8" s="1" t="n"/>
-      <c r="J8" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="K8" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="L8" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="I8" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="J8" s="1" t="n"/>
+      <c r="K8" s="1" t="n"/>
+      <c r="L8" s="1" t="n"/>
       <c r="M8" s="1" t="n"/>
-      <c r="N8" s="1" t="n"/>
+      <c r="N8" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="O8" s="1" t="n"/>
       <c r="P8" s="1" t="n"/>
       <c r="Q8" s="1" t="n"/>
@@ -878,37 +878,37 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C9" s="1" t="n"/>
-      <c r="D9" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="n"/>
-      <c r="F9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="G9" s="1" t="n"/>
       <c r="H9" s="1" t="n"/>
-      <c r="I9" s="1" t="n"/>
-      <c r="J9" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="K9" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="L9" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="I9" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="J9" s="1" t="n"/>
+      <c r="K9" s="1" t="n"/>
+      <c r="L9" s="1" t="n"/>
       <c r="M9" s="1" t="n"/>
-      <c r="N9" s="1" t="n"/>
+      <c r="N9" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="O9" s="1" t="n"/>
       <c r="P9" s="1" t="n"/>
       <c r="Q9" s="1" t="n"/>
@@ -928,39 +928,39 @@
         </is>
       </c>
       <c r="B10" s="1" t="n"/>
-      <c r="C10" s="1" t="n"/>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="D10" s="1" t="n"/>
       <c r="E10" s="1" t="n"/>
-      <c r="F10" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="G10" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="F10" s="1" t="n"/>
+      <c r="G10" s="1" t="n"/>
       <c r="H10" s="1" t="inlineStr">
         <is>
-          <t>CCTV2</t>
+          <t>VACS</t>
         </is>
       </c>
       <c r="I10" s="1" t="n"/>
-      <c r="J10" s="1" t="n"/>
+      <c r="J10" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="K10" s="1" t="n"/>
-      <c r="L10" s="1" t="n"/>
+      <c r="L10" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="M10" s="1" t="n"/>
       <c r="N10" s="1" t="n"/>
       <c r="O10" s="1" t="n"/>
-      <c r="P10" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="P10" s="1" t="n"/>
       <c r="Q10" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>CCTV</t>
         </is>
       </c>
       <c r="R10" s="1" t="inlineStr">
@@ -979,39 +979,39 @@
         </is>
       </c>
       <c r="B11" s="1" t="n"/>
-      <c r="C11" s="1" t="n"/>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="D11" s="1" t="n"/>
       <c r="E11" s="1" t="n"/>
-      <c r="F11" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="G11" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" s="1" t="n"/>
       <c r="H11" s="1" t="inlineStr">
         <is>
-          <t>CCTV2</t>
+          <t>VACS</t>
         </is>
       </c>
       <c r="I11" s="1" t="n"/>
-      <c r="J11" s="1" t="n"/>
+      <c r="J11" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="K11" s="1" t="n"/>
-      <c r="L11" s="1" t="n"/>
+      <c r="L11" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="M11" s="1" t="n"/>
       <c r="N11" s="1" t="n"/>
       <c r="O11" s="1" t="n"/>
-      <c r="P11" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="P11" s="1" t="n"/>
       <c r="Q11" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>CCTV</t>
         </is>
       </c>
       <c r="R11" s="1" t="inlineStr">
@@ -1029,38 +1029,38 @@
           <t>0700-0900</t>
         </is>
       </c>
-      <c r="B12" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="B12" s="1" t="n"/>
       <c r="C12" s="1" t="n"/>
       <c r="D12" s="1" t="n"/>
-      <c r="E12" s="1" t="n"/>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="F12" s="1" t="n"/>
-      <c r="G12" s="1" t="n"/>
+      <c r="G12" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="H12" s="1" t="n"/>
       <c r="I12" s="1" t="n"/>
       <c r="J12" s="1" t="n"/>
       <c r="K12" s="1" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>TG</t>
         </is>
       </c>
       <c r="L12" s="1" t="n"/>
       <c r="M12" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="N12" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="N12" s="1" t="n"/>
       <c r="O12" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>CCTV</t>
         </is>
       </c>
       <c r="P12" s="1" t="n"/>
@@ -1080,38 +1080,38 @@
           <t>0900-1100</t>
         </is>
       </c>
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="B13" s="1" t="n"/>
       <c r="C13" s="1" t="n"/>
       <c r="D13" s="1" t="n"/>
-      <c r="E13" s="1" t="n"/>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="F13" s="1" t="n"/>
-      <c r="G13" s="1" t="n"/>
+      <c r="G13" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="H13" s="1" t="n"/>
       <c r="I13" s="1" t="n"/>
       <c r="J13" s="1" t="n"/>
       <c r="K13" s="1" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>TG</t>
         </is>
       </c>
       <c r="L13" s="1" t="n"/>
       <c r="M13" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="N13" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="N13" s="1" t="n"/>
       <c r="O13" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>CCTV</t>
         </is>
       </c>
       <c r="P13" s="1" t="n"/>
@@ -1131,41 +1131,41 @@
           <t>1100-1300</t>
         </is>
       </c>
-      <c r="B14" s="1" t="n"/>
-      <c r="C14" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="n"/>
       <c r="D14" s="1" t="inlineStr">
         <is>
           <t>TG</t>
         </is>
       </c>
-      <c r="E14" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="E14" s="1" t="n"/>
       <c r="F14" s="1" t="n"/>
       <c r="G14" s="1" t="n"/>
       <c r="H14" s="1" t="n"/>
-      <c r="I14" s="1" t="n"/>
+      <c r="I14" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="J14" s="1" t="n"/>
       <c r="K14" s="1" t="n"/>
       <c r="L14" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
+          <t>CCTV2</t>
         </is>
       </c>
       <c r="M14" s="1" t="n"/>
-      <c r="N14" s="1" t="n"/>
+      <c r="N14" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="O14" s="1" t="n"/>
-      <c r="P14" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="P14" s="1" t="n"/>
       <c r="Q14" s="1" t="n"/>
       <c r="R14" s="1" t="inlineStr">
         <is>
@@ -1182,41 +1182,41 @@
           <t>1300-1500</t>
         </is>
       </c>
-      <c r="B15" s="1" t="n"/>
-      <c r="C15" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="n"/>
       <c r="D15" s="1" t="inlineStr">
         <is>
           <t>TG</t>
         </is>
       </c>
-      <c r="E15" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="E15" s="1" t="n"/>
       <c r="F15" s="1" t="n"/>
       <c r="G15" s="1" t="n"/>
       <c r="H15" s="1" t="n"/>
-      <c r="I15" s="1" t="n"/>
+      <c r="I15" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="J15" s="1" t="n"/>
       <c r="K15" s="1" t="n"/>
       <c r="L15" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
+          <t>CCTV2</t>
         </is>
       </c>
       <c r="M15" s="1" t="n"/>
-      <c r="N15" s="1" t="n"/>
+      <c r="N15" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="O15" s="1" t="n"/>
-      <c r="P15" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="P15" s="1" t="n"/>
       <c r="Q15" s="1" t="n"/>
       <c r="R15" s="1" t="inlineStr">
         <is>
@@ -1234,41 +1234,41 @@
         </is>
       </c>
       <c r="B16" s="1" t="n"/>
-      <c r="C16" s="1" t="n"/>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="D16" s="1" t="n"/>
-      <c r="E16" s="1" t="n"/>
-      <c r="F16" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="n"/>
       <c r="G16" s="1" t="inlineStr">
         <is>
-          <t>CCTV2</t>
+          <t>18</t>
         </is>
       </c>
       <c r="H16" s="1" t="n"/>
-      <c r="I16" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="I16" s="1" t="n"/>
       <c r="J16" s="1" t="n"/>
       <c r="K16" s="1" t="n"/>
       <c r="L16" s="1" t="n"/>
       <c r="M16" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>CCTV</t>
         </is>
       </c>
       <c r="N16" s="1" t="n"/>
-      <c r="O16" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="O16" s="1" t="n"/>
       <c r="P16" s="1" t="n"/>
-      <c r="Q16" s="1" t="n"/>
+      <c r="Q16" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="R16" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1285,41 +1285,41 @@
         </is>
       </c>
       <c r="B17" s="1" t="n"/>
-      <c r="C17" s="1" t="n"/>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="D17" s="1" t="n"/>
-      <c r="E17" s="1" t="n"/>
-      <c r="F17" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="E17" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="F17" s="1" t="n"/>
       <c r="G17" s="1" t="inlineStr">
         <is>
-          <t>CCTV2</t>
+          <t>18</t>
         </is>
       </c>
       <c r="H17" s="1" t="n"/>
-      <c r="I17" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="I17" s="1" t="n"/>
       <c r="J17" s="1" t="n"/>
       <c r="K17" s="1" t="n"/>
       <c r="L17" s="1" t="n"/>
       <c r="M17" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>CCTV</t>
         </is>
       </c>
       <c r="N17" s="1" t="n"/>
-      <c r="O17" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="O17" s="1" t="n"/>
       <c r="P17" s="1" t="n"/>
-      <c r="Q17" s="1" t="n"/>
+      <c r="Q17" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="R17" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1335,42 +1335,42 @@
           <t>1900-2100</t>
         </is>
       </c>
-      <c r="B18" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="B18" s="1" t="n"/>
       <c r="C18" s="1" t="n"/>
-      <c r="D18" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
+      <c r="D18" s="1" t="n"/>
       <c r="E18" s="1" t="n"/>
       <c r="F18" s="1" t="n"/>
       <c r="G18" s="1" t="n"/>
       <c r="H18" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="I18" s="1" t="n"/>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="I18" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="J18" s="1" t="n"/>
       <c r="K18" s="1" t="n"/>
-      <c r="L18" s="1" t="n"/>
+      <c r="L18" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="M18" s="1" t="n"/>
-      <c r="N18" s="1" t="n"/>
+      <c r="N18" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="O18" s="1" t="n"/>
       <c r="P18" s="1" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="Q18" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="Q18" s="1" t="n"/>
       <c r="R18" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1386,42 +1386,42 @@
           <t>2100-2300</t>
         </is>
       </c>
-      <c r="B19" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="B19" s="1" t="n"/>
       <c r="C19" s="1" t="n"/>
-      <c r="D19" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
+      <c r="D19" s="1" t="n"/>
       <c r="E19" s="1" t="n"/>
       <c r="F19" s="1" t="n"/>
       <c r="G19" s="1" t="n"/>
       <c r="H19" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="I19" s="1" t="n"/>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="I19" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="J19" s="1" t="n"/>
       <c r="K19" s="1" t="n"/>
-      <c r="L19" s="1" t="n"/>
+      <c r="L19" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="M19" s="1" t="n"/>
-      <c r="N19" s="1" t="n"/>
+      <c r="N19" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="O19" s="1" t="n"/>
       <c r="P19" s="1" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="Q19" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="Q19" s="1" t="n"/>
       <c r="R19" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1440,39 +1440,39 @@
       <c r="B20" s="1" t="n"/>
       <c r="C20" s="1" t="n"/>
       <c r="D20" s="1" t="n"/>
-      <c r="E20" s="1" t="n"/>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="F20" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
+          <t>18</t>
         </is>
       </c>
       <c r="G20" s="1" t="n"/>
       <c r="H20" s="1" t="n"/>
-      <c r="I20" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="J20" s="1" t="n"/>
+      <c r="I20" s="1" t="n"/>
+      <c r="J20" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="K20" s="1" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="L20" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="L20" s="1" t="n"/>
       <c r="M20" s="1" t="n"/>
       <c r="N20" s="1" t="n"/>
-      <c r="O20" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
+      <c r="O20" s="1" t="n"/>
       <c r="P20" s="1" t="n"/>
-      <c r="Q20" s="1" t="n"/>
+      <c r="Q20" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="R20" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1491,39 +1491,39 @@
       <c r="B21" s="1" t="n"/>
       <c r="C21" s="1" t="n"/>
       <c r="D21" s="1" t="n"/>
-      <c r="E21" s="1" t="n"/>
+      <c r="E21" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="F21" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
+          <t>18</t>
         </is>
       </c>
       <c r="G21" s="1" t="n"/>
       <c r="H21" s="1" t="n"/>
-      <c r="I21" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="J21" s="1" t="n"/>
+      <c r="I21" s="1" t="n"/>
+      <c r="J21" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="K21" s="1" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="L21" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="L21" s="1" t="n"/>
       <c r="M21" s="1" t="n"/>
       <c r="N21" s="1" t="n"/>
-      <c r="O21" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
+      <c r="O21" s="1" t="n"/>
       <c r="P21" s="1" t="n"/>
-      <c r="Q21" s="1" t="n"/>
+      <c r="Q21" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="R21" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1541,39 +1541,39 @@
       </c>
       <c r="B22" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="C22" s="1" t="n"/>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="D22" s="1" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="E22" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="n"/>
       <c r="F22" s="1" t="n"/>
-      <c r="G22" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="H22" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="G22" s="1" t="n"/>
+      <c r="H22" s="1" t="n"/>
       <c r="I22" s="1" t="n"/>
       <c r="J22" s="1" t="n"/>
       <c r="K22" s="1" t="n"/>
       <c r="L22" s="1" t="n"/>
       <c r="M22" s="1" t="n"/>
-      <c r="N22" s="1" t="n"/>
+      <c r="N22" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="O22" s="1" t="n"/>
-      <c r="P22" s="1" t="n"/>
+      <c r="P22" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="Q22" s="1" t="n"/>
       <c r="R22" s="1" t="inlineStr">
         <is>
@@ -1592,39 +1592,39 @@
       </c>
       <c r="B23" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="C23" s="1" t="n"/>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="E23" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="E23" s="1" t="n"/>
       <c r="F23" s="1" t="n"/>
-      <c r="G23" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="H23" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="G23" s="1" t="n"/>
+      <c r="H23" s="1" t="n"/>
       <c r="I23" s="1" t="n"/>
       <c r="J23" s="1" t="n"/>
       <c r="K23" s="1" t="n"/>
       <c r="L23" s="1" t="n"/>
       <c r="M23" s="1" t="n"/>
-      <c r="N23" s="1" t="n"/>
+      <c r="N23" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="O23" s="1" t="n"/>
-      <c r="P23" s="1" t="n"/>
+      <c r="P23" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="Q23" s="1" t="n"/>
       <c r="R23" s="1" t="inlineStr">
         <is>
@@ -1644,39 +1644,39 @@
       <c r="B24" s="1" t="n"/>
       <c r="C24" s="1" t="n"/>
       <c r="D24" s="1" t="n"/>
-      <c r="E24" s="1" t="n"/>
-      <c r="F24" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="G24" s="1" t="n"/>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="n"/>
+      <c r="G24" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="H24" s="1" t="n"/>
       <c r="I24" s="1" t="n"/>
       <c r="J24" s="1" t="inlineStr">
         <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="K24" s="1" t="n"/>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="K24" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
       <c r="L24" s="1" t="inlineStr">
         <is>
-          <t>CCTV2</t>
+          <t>VACS</t>
         </is>
       </c>
       <c r="M24" s="1" t="n"/>
-      <c r="N24" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="N24" s="1" t="n"/>
       <c r="O24" s="1" t="n"/>
       <c r="P24" s="1" t="n"/>
-      <c r="Q24" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="Q24" s="1" t="n"/>
       <c r="R24" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1695,39 +1695,39 @@
       <c r="B25" s="1" t="n"/>
       <c r="C25" s="1" t="n"/>
       <c r="D25" s="1" t="n"/>
-      <c r="E25" s="1" t="n"/>
-      <c r="F25" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="G25" s="1" t="n"/>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="n"/>
+      <c r="G25" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="H25" s="1" t="n"/>
       <c r="I25" s="1" t="n"/>
       <c r="J25" s="1" t="inlineStr">
         <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="K25" s="1" t="n"/>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="K25" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
       <c r="L25" s="1" t="inlineStr">
         <is>
-          <t>CCTV2</t>
+          <t>VACS</t>
         </is>
       </c>
       <c r="M25" s="1" t="n"/>
-      <c r="N25" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+      <c r="N25" s="1" t="n"/>
       <c r="O25" s="1" t="n"/>
       <c r="P25" s="1" t="n"/>
-      <c r="Q25" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="Q25" s="1" t="n"/>
       <c r="R25" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1747,7 +1747,7 @@
       <c r="C26" s="1" t="n"/>
       <c r="D26" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>VACS</t>
         </is>
       </c>
       <c r="E26" s="1" t="n"/>
@@ -1755,30 +1755,30 @@
       <c r="G26" s="1" t="n"/>
       <c r="H26" s="1" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>CCTV</t>
         </is>
       </c>
       <c r="I26" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
+          <t>18</t>
         </is>
       </c>
       <c r="J26" s="1" t="n"/>
-      <c r="K26" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="K26" s="1" t="n"/>
       <c r="L26" s="1" t="n"/>
       <c r="M26" s="1" t="inlineStr">
         <is>
-          <t>VACS</t>
+          <t>CCTV2</t>
         </is>
       </c>
       <c r="N26" s="1" t="n"/>
       <c r="O26" s="1" t="n"/>
       <c r="P26" s="1" t="n"/>
-      <c r="Q26" s="1" t="n"/>
+      <c r="Q26" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="R26" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1798,7 +1798,7 @@
       <c r="C27" s="1" t="n"/>
       <c r="D27" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>VACS</t>
         </is>
       </c>
       <c r="E27" s="1" t="n"/>
@@ -1806,30 +1806,30 @@
       <c r="G27" s="1" t="n"/>
       <c r="H27" s="1" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>CCTV</t>
         </is>
       </c>
       <c r="I27" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
+          <t>18</t>
         </is>
       </c>
       <c r="J27" s="1" t="n"/>
-      <c r="K27" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="K27" s="1" t="n"/>
       <c r="L27" s="1" t="n"/>
       <c r="M27" s="1" t="inlineStr">
         <is>
-          <t>VACS</t>
+          <t>CCTV2</t>
         </is>
       </c>
       <c r="N27" s="1" t="n"/>
       <c r="O27" s="1" t="n"/>
       <c r="P27" s="1" t="n"/>
-      <c r="Q27" s="1" t="n"/>
+      <c r="Q27" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="R27" s="1" t="inlineStr">
         <is>
           <t>STAYOUT</t>
@@ -1845,41 +1845,41 @@
           <t>1500-1700</t>
         </is>
       </c>
-      <c r="B28" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="C28" s="1" t="n"/>
+      <c r="B28" s="1" t="n"/>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
       <c r="D28" s="1" t="n"/>
-      <c r="E28" s="1" t="n"/>
-      <c r="F28" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="G28" s="1" t="n"/>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="n"/>
+      <c r="G28" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="H28" s="1" t="n"/>
       <c r="I28" s="1" t="n"/>
-      <c r="J28" s="1" t="n"/>
+      <c r="J28" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="K28" s="1" t="n"/>
       <c r="L28" s="1" t="n"/>
       <c r="M28" s="1" t="n"/>
       <c r="N28" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="O28" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="P28" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="O28" s="1" t="n"/>
+      <c r="P28" s="1" t="n"/>
       <c r="Q28" s="1" t="n"/>
       <c r="R28" s="1" t="inlineStr">
         <is>
@@ -1896,41 +1896,41 @@
           <t>1700-1900</t>
         </is>
       </c>
-      <c r="B29" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="C29" s="1" t="n"/>
+      <c r="B29" s="1" t="n"/>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
       <c r="D29" s="1" t="n"/>
-      <c r="E29" s="1" t="n"/>
-      <c r="F29" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="G29" s="1" t="n"/>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="n"/>
+      <c r="G29" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="H29" s="1" t="n"/>
       <c r="I29" s="1" t="n"/>
-      <c r="J29" s="1" t="n"/>
+      <c r="J29" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="K29" s="1" t="n"/>
       <c r="L29" s="1" t="n"/>
       <c r="M29" s="1" t="n"/>
       <c r="N29" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
-        </is>
-      </c>
-      <c r="O29" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="P29" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+          <t>VACS</t>
+        </is>
+      </c>
+      <c r="O29" s="1" t="n"/>
+      <c r="P29" s="1" t="n"/>
       <c r="Q29" s="1" t="n"/>
       <c r="R29" s="1" t="inlineStr">
         <is>
@@ -1951,36 +1951,36 @@
       <c r="C30" s="1" t="n"/>
       <c r="D30" s="1" t="n"/>
       <c r="E30" s="1" t="n"/>
-      <c r="F30" s="1" t="n"/>
+      <c r="F30" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="G30" s="1" t="n"/>
-      <c r="H30" s="1" t="n"/>
-      <c r="I30" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="H30" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="I30" s="1" t="n"/>
       <c r="J30" s="1" t="n"/>
-      <c r="K30" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="K30" s="1" t="n"/>
       <c r="L30" s="1" t="inlineStr">
         <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="M30" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="M30" s="1" t="n"/>
       <c r="N30" s="1" t="n"/>
       <c r="O30" s="1" t="n"/>
-      <c r="P30" s="1" t="n"/>
+      <c r="P30" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="Q30" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>18</t>
         </is>
       </c>
       <c r="R30" s="1" t="inlineStr">
@@ -2002,36 +2002,36 @@
       <c r="C31" s="1" t="n"/>
       <c r="D31" s="1" t="n"/>
       <c r="E31" s="1" t="n"/>
-      <c r="F31" s="1" t="n"/>
+      <c r="F31" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
       <c r="G31" s="1" t="n"/>
-      <c r="H31" s="1" t="n"/>
-      <c r="I31" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="H31" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
+      <c r="I31" s="1" t="n"/>
       <c r="J31" s="1" t="n"/>
-      <c r="K31" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="K31" s="1" t="n"/>
       <c r="L31" s="1" t="inlineStr">
         <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="M31" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="M31" s="1" t="n"/>
       <c r="N31" s="1" t="n"/>
       <c r="O31" s="1" t="n"/>
-      <c r="P31" s="1" t="n"/>
+      <c r="P31" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="Q31" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>18</t>
         </is>
       </c>
       <c r="R31" s="1" t="inlineStr">
@@ -2050,40 +2050,40 @@
         </is>
       </c>
       <c r="B32" s="1" t="n"/>
-      <c r="C32" s="1" t="n"/>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="D32" s="1" t="n"/>
-      <c r="E32" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="E32" s="1" t="n"/>
       <c r="F32" s="1" t="n"/>
-      <c r="G32" s="1" t="n"/>
+      <c r="G32" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="H32" s="1" t="n"/>
-      <c r="I32" s="1" t="n"/>
+      <c r="I32" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
       <c r="J32" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>18</t>
         </is>
       </c>
       <c r="K32" s="1" t="n"/>
       <c r="L32" s="1" t="n"/>
-      <c r="M32" s="1" t="n"/>
-      <c r="N32" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O32" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="P32" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="M32" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="N32" s="1" t="n"/>
+      <c r="O32" s="1" t="n"/>
+      <c r="P32" s="1" t="n"/>
       <c r="Q32" s="1" t="n"/>
       <c r="R32" s="1" t="inlineStr">
         <is>
@@ -2101,40 +2101,40 @@
         </is>
       </c>
       <c r="B33" s="1" t="n"/>
-      <c r="C33" s="1" t="n"/>
+      <c r="C33" s="1" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="D33" s="1" t="n"/>
-      <c r="E33" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="E33" s="1" t="n"/>
       <c r="F33" s="1" t="n"/>
-      <c r="G33" s="1" t="n"/>
+      <c r="G33" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="H33" s="1" t="n"/>
-      <c r="I33" s="1" t="n"/>
+      <c r="I33" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
       <c r="J33" s="1" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>18</t>
         </is>
       </c>
       <c r="K33" s="1" t="n"/>
       <c r="L33" s="1" t="n"/>
-      <c r="M33" s="1" t="n"/>
-      <c r="N33" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="O33" s="1" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
-      <c r="P33" s="1" t="inlineStr">
-        <is>
-          <t>CCTV</t>
-        </is>
-      </c>
+      <c r="M33" s="1" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="N33" s="1" t="n"/>
+      <c r="O33" s="1" t="n"/>
+      <c r="P33" s="1" t="n"/>
       <c r="Q33" s="1" t="n"/>
       <c r="R33" s="1" t="inlineStr">
         <is>
@@ -2151,19 +2151,19 @@
           <t>0300-0500</t>
         </is>
       </c>
-      <c r="B34" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="B34" s="1" t="n"/>
       <c r="C34" s="1" t="n"/>
-      <c r="D34" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="E34" s="1" t="n"/>
-      <c r="F34" s="1" t="n"/>
+      <c r="D34" s="1" t="n"/>
+      <c r="E34" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="F34" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="G34" s="1" t="n"/>
       <c r="H34" s="1" t="n"/>
       <c r="I34" s="1" t="n"/>
@@ -2171,20 +2171,20 @@
       <c r="K34" s="1" t="n"/>
       <c r="L34" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="M34" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="M34" s="1" t="n"/>
       <c r="N34" s="1" t="n"/>
       <c r="O34" s="1" t="n"/>
-      <c r="P34" s="1" t="n"/>
+      <c r="P34" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="Q34" s="1" t="inlineStr">
         <is>
-          <t>VACS</t>
+          <t>TG</t>
         </is>
       </c>
       <c r="R34" s="1" t="inlineStr">
@@ -2202,19 +2202,19 @@
           <t>0500-0700</t>
         </is>
       </c>
-      <c r="B35" s="1" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
+      <c r="B35" s="1" t="n"/>
       <c r="C35" s="1" t="n"/>
-      <c r="D35" s="1" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="E35" s="1" t="n"/>
-      <c r="F35" s="1" t="n"/>
+      <c r="D35" s="1" t="n"/>
+      <c r="E35" s="1" t="inlineStr">
+        <is>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="F35" s="1" t="inlineStr">
+        <is>
+          <t>VACS</t>
+        </is>
+      </c>
       <c r="G35" s="1" t="n"/>
       <c r="H35" s="1" t="n"/>
       <c r="I35" s="1" t="n"/>
@@ -2222,20 +2222,20 @@
       <c r="K35" s="1" t="n"/>
       <c r="L35" s="1" t="inlineStr">
         <is>
-          <t>CCTV</t>
-        </is>
-      </c>
-      <c r="M35" s="1" t="inlineStr">
-        <is>
-          <t>TG</t>
-        </is>
-      </c>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="M35" s="1" t="n"/>
       <c r="N35" s="1" t="n"/>
       <c r="O35" s="1" t="n"/>
-      <c r="P35" s="1" t="n"/>
+      <c r="P35" s="1" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
       <c r="Q35" s="1" t="inlineStr">
         <is>
-          <t>VACS</t>
+          <t>TG</t>
         </is>
       </c>
       <c r="R35" s="1" t="inlineStr">
@@ -2253,32 +2253,32 @@
           <t>0700-0900</t>
         </is>
       </c>
-      <c r="B36" s="2" t="n"/>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>XSVC2</t>
+        </is>
+      </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="D36" s="2" t="n"/>
-      <c r="E36" s="2" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="F36" s="2" t="inlineStr">
-        <is>
           <t>CHKR</t>
         </is>
       </c>
-      <c r="G36" s="2" t="n"/>
-      <c r="H36" s="2" t="inlineStr">
-        <is>
-          <t>VACS</t>
-        </is>
-      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="n"/>
+      <c r="F36" s="2" t="n"/>
+      <c r="G36" s="2" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
+        </is>
+      </c>
+      <c r="H36" s="2" t="n"/>
       <c r="I36" s="2" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>VACS</t>
         </is>
       </c>
       <c r="J36" s="2" t="inlineStr">
@@ -2288,26 +2288,26 @@
       </c>
       <c r="K36" s="2" t="inlineStr">
         <is>
-          <t>CCTV</t>
+          <t>XCBT</t>
         </is>
       </c>
       <c r="L36" s="2" t="n"/>
-      <c r="M36" s="2" t="n"/>
+      <c r="M36" s="2" t="inlineStr">
+        <is>
+          <t>TG</t>
+        </is>
+      </c>
       <c r="N36" s="2" t="inlineStr">
         <is>
-          <t>XSVC2</t>
+          <t>TG2</t>
         </is>
       </c>
       <c r="O36" s="2" t="inlineStr">
         <is>
-          <t>XCBT</t>
-        </is>
-      </c>
-      <c r="P36" s="2" t="inlineStr">
-        <is>
-          <t>TG2</t>
-        </is>
-      </c>
+          <t>CCTV</t>
+        </is>
+      </c>
+      <c r="P36" s="2" t="n"/>
       <c r="Q36" s="2" t="n"/>
       <c r="R36" s="2" t="n"/>
       <c r="S36" s="2" t="n">
@@ -2320,24 +2320,19 @@
           <t>0900-1100</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>CCTV2</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>VACS</t>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>CCTV2</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>TG</t>
+          <t>VACS</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2347,12 +2342,17 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>CCTV</t>
+          <t>XCBT</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>TG</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>XCBT</t>
+          <t>CCTV</t>
         </is>
       </c>
       <c r="S37" t="n">
@@ -2366,55 +2366,55 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C38" t="n">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D38" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E38" t="n">
+        <v>32</v>
+      </c>
+      <c r="F38" t="n">
         <v>20</v>
       </c>
-      <c r="F38" t="n">
-        <v>30</v>
-      </c>
       <c r="G38" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H38" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="I38" t="n">
         <v>28</v>
       </c>
       <c r="J38" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K38" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="L38" t="n">
         <v>28</v>
       </c>
       <c r="M38" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="N38" t="n">
         <v>26</v>
       </c>
       <c r="O38" t="n">
+        <v>12</v>
+      </c>
+      <c r="P38" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q38" t="n">
         <v>28</v>
       </c>
-      <c r="P38" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>24</v>
-      </c>
       <c r="R38" t="n">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>